<commit_message>
Mathematica plot bond angles
</commit_message>
<xml_diff>
--- a/Viscosity Testing - Green-Kubo.xlsx
+++ b/Viscosity Testing - Green-Kubo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Particles" sheetId="11" r:id="rId1"/>
@@ -17,10 +17,11 @@
     <sheet name="Particles 10x Time" sheetId="6" r:id="rId3"/>
     <sheet name="Particles Remove Wat" sheetId="13" r:id="rId4"/>
     <sheet name="Particles Remove Wat 0.1x Step" sheetId="14" r:id="rId5"/>
+    <sheet name="Difference" sheetId="15" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="0" hidden="1">Particles!$J$58</definedName>
-    <definedName name="solver_adj" localSheetId="2" hidden="1">'Particles 10x Time'!$J$58:$J$60</definedName>
+    <definedName name="solver_adj" localSheetId="2" hidden="1">'Particles 10x Time'!$J$58</definedName>
     <definedName name="solver_adj" localSheetId="1" hidden="1">'Particles 5x E_CC'!$J$58:$J$60</definedName>
     <definedName name="solver_adj" localSheetId="3" hidden="1">'Particles Remove Wat'!$AF$52</definedName>
     <definedName name="solver_adj" localSheetId="4" hidden="1">'Particles Remove Wat 0.1x Step'!$AG$52</definedName>
@@ -195,7 +196,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="77">
   <si>
     <t>1. N_WATER</t>
   </si>
@@ -403,6 +404,30 @@
   <si>
     <t>d</t>
   </si>
+  <si>
+    <t>Difference compared to the Shear LE</t>
+  </si>
+  <si>
+    <t>* 0 shear vs approx 0.1 shear</t>
+  </si>
+  <si>
+    <t>* Moment of inertia differences</t>
+  </si>
+  <si>
+    <t>* 0.3 for water vs 2/5 MR^2 = 0.1</t>
+  </si>
+  <si>
+    <t>* 289.15 for particles vs 2/5 MR^2 = 490.75</t>
+  </si>
+  <si>
+    <t>* Interaction distance (sigma - eq. distance for LJ potential)</t>
+  </si>
+  <si>
+    <t>* 2.45 for water-colloid vs 0.8 x distance = 0.8 x (2.5 + 0.5) = 2.4</t>
+  </si>
+  <si>
+    <t>* 4.45 for colloid-colloid vs 0.9 x distance = 0.9 x (2.5 + 2.5) = 4.5</t>
+  </si>
 </sst>
 </file>
 
@@ -571,6 +596,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1175,6 +1201,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1297,6 +1324,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1591,71 +1619,17 @@
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="11">
                   <c:v>43.32863227604436</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="14">
                   <c:v>50.877815606504619</c:v>
                 </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="17">
                   <c:v>64.317143595931725</c:v>
                 </c:pt>
-                <c:pt idx="18">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="20">
                   <c:v>70.67396785037063</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>134.21600083318967</c:v>
@@ -1865,106 +1839,106 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0368774959931355</c:v>
+                  <c:v>1.0301893897675021</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.1742415121718948</c:v>
+                  <c:v>1.0962416171645919</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5680794373436795</c:v>
+                  <c:v>1.2119640307752102</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.2432919345776541</c:v>
+                  <c:v>1.3526120008408742</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.2803791987232569</c:v>
+                  <c:v>1.525646867927472</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.785248297621723</c:v>
+                  <c:v>1.7415073549536146</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.8987427786497859</c:v>
+                  <c:v>2.0151478038015225</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.8104562528729033</c:v>
+                  <c:v>2.3685862490418956</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>13.779130521396597</c:v>
+                  <c:v>2.8352955296716074</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>19.163407336613755</c:v>
+                  <c:v>3.4681304939327204</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>26.469281139594774</c:v>
+                  <c:v>4.3544548615869676</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>29.449093448705653</c:v>
+                  <c:v>4.7297584036803864</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>32.754773407760844</c:v>
+                  <c:v>5.1572740816545934</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>36.425278318672731</c:v>
+                  <c:v>5.6470195462680248</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>40.505159797121827</c:v>
+                  <c:v>6.2115218420437621</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>45.045526038285914</c:v>
+                  <c:v>6.8666091366086244</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>50.105199617956551</c:v>
+                  <c:v>7.632509479469844</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>55.752117131314037</c:v>
+                  <c:v>8.5354004548607314</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>62.065029599807239</c:v>
+                  <c:v>9.6096340654112424</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>69.135579133252619</c:v>
+                  <c:v>10.90099493757957</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>77.070849202300593</c:v>
+                  <c:v>12.471578501343851</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>85.996514985951606</c:v>
+                  <c:v>14.407278658280561</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>96.060759329278596</c:v>
+                  <c:v>16.829609750345881</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>107.43917274810902</c:v>
+                  <c:v>19.914983935992684</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>120.34092821668052</c:v>
+                  <c:v>23.927339732875247</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>135.01662126874359</c:v>
+                  <c:v>29.275828968053169</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>151.76830515398774</c:v>
+                  <c:v>36.622216837623625</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>170.96244719918877</c:v>
+                  <c:v>47.093700304889502</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>193.04681300848333</c:v>
+                  <c:v>62.738294836510747</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>218.57269094736108</c:v>
+                  <c:v>87.598833272317279</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>248.22446479430565</c:v>
+                  <c:v>130.59111722045046</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>282.85942949143924</c:v>
+                  <c:v>214.70712689046451</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>323.56208833184695</c:v>
+                  <c:v>415.35438948145787</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>371.71924125522042</c:v>
+                  <c:v>1112.8271490493012</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8553,6 +8527,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8639,6 +8614,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -10544,6 +10520,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10583,15 +10560,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>'Particles 5x E_CC'!$L$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>V_norm_1k_5x</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Epsilon = 550</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -10622,228 +10591,126 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>'Particles 5x E_CC'!$M$2:$M$36</c:f>
+                <c:f>('Particles 5x E_CC'!$M$2,'Particles 5x E_CC'!$M$17:$M$33)</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="35"/>
+                  <c:ptCount val="18"/>
                   <c:pt idx="0">
                     <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0</c:v>
+                    <c:v>19.218992607022866</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0</c:v>
+                    <c:v>13.491901440955241</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0</c:v>
+                    <c:v>62.85622791711603</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0</c:v>
+                    <c:v>97.264362087705166</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0</c:v>
+                    <c:v>0.13670495400679744</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0</c:v>
+                    <c:v>42.000014411069273</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>0</c:v>
+                    <c:v>14.22536916294443</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>0</c:v>
+                    <c:v>204.80327561983091</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>0</c:v>
+                    <c:v>21.394873309818859</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>0</c:v>
+                    <c:v>37.027342540917701</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>0</c:v>
+                    <c:v>333.42559606679862</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>0</c:v>
+                    <c:v>87.362936749580342</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>0</c:v>
+                    <c:v>177.02776770143288</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>0</c:v>
+                    <c:v>199.81879506643384</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>19.218992607022866</c:v>
+                    <c:v>379.22121118685305</c:v>
                   </c:pt>
                   <c:pt idx="16">
-                    <c:v>13.491901440955241</c:v>
+                    <c:v>144.76850275459859</c:v>
                   </c:pt>
                   <c:pt idx="17">
-                    <c:v>62.85622791711603</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v>97.264362087705166</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
-                    <c:v>0.13670495400679744</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>42.000014411069273</c:v>
-                  </c:pt>
-                  <c:pt idx="21">
-                    <c:v>14.22536916294443</c:v>
-                  </c:pt>
-                  <c:pt idx="22">
-                    <c:v>204.80327561983091</c:v>
-                  </c:pt>
-                  <c:pt idx="23">
-                    <c:v>21.394873309818859</c:v>
-                  </c:pt>
-                  <c:pt idx="24">
-                    <c:v>37.027342540917701</c:v>
-                  </c:pt>
-                  <c:pt idx="25">
-                    <c:v>333.42559606679862</c:v>
-                  </c:pt>
-                  <c:pt idx="26">
-                    <c:v>87.362936749580342</c:v>
-                  </c:pt>
-                  <c:pt idx="27">
-                    <c:v>177.02776770143288</c:v>
-                  </c:pt>
-                  <c:pt idx="28">
-                    <c:v>199.81879506643384</c:v>
-                  </c:pt>
-                  <c:pt idx="29">
-                    <c:v>379.22121118685305</c:v>
-                  </c:pt>
-                  <c:pt idx="30">
-                    <c:v>144.76850275459859</c:v>
-                  </c:pt>
-                  <c:pt idx="31">
                     <c:v>1230.3773463183302</c:v>
-                  </c:pt>
-                  <c:pt idx="32">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="33">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="34">
-                    <c:v>0</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>'Particles 5x E_CC'!$M$2:$M$36</c:f>
+                <c:f>('Particles 5x E_CC'!$M$2,'Particles 5x E_CC'!$M$17:$M$33)</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="35"/>
+                  <c:ptCount val="18"/>
                   <c:pt idx="0">
                     <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0</c:v>
+                    <c:v>19.218992607022866</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0</c:v>
+                    <c:v>13.491901440955241</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0</c:v>
+                    <c:v>62.85622791711603</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0</c:v>
+                    <c:v>97.264362087705166</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0</c:v>
+                    <c:v>0.13670495400679744</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0</c:v>
+                    <c:v>42.000014411069273</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>0</c:v>
+                    <c:v>14.22536916294443</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>0</c:v>
+                    <c:v>204.80327561983091</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>0</c:v>
+                    <c:v>21.394873309818859</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>0</c:v>
+                    <c:v>37.027342540917701</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>0</c:v>
+                    <c:v>333.42559606679862</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>0</c:v>
+                    <c:v>87.362936749580342</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>0</c:v>
+                    <c:v>177.02776770143288</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>0</c:v>
+                    <c:v>199.81879506643384</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>19.218992607022866</c:v>
+                    <c:v>379.22121118685305</c:v>
                   </c:pt>
                   <c:pt idx="16">
-                    <c:v>13.491901440955241</c:v>
+                    <c:v>144.76850275459859</c:v>
                   </c:pt>
                   <c:pt idx="17">
-                    <c:v>62.85622791711603</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v>97.264362087705166</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
-                    <c:v>0.13670495400679744</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>42.000014411069273</c:v>
-                  </c:pt>
-                  <c:pt idx="21">
-                    <c:v>14.22536916294443</c:v>
-                  </c:pt>
-                  <c:pt idx="22">
-                    <c:v>204.80327561983091</c:v>
-                  </c:pt>
-                  <c:pt idx="23">
-                    <c:v>21.394873309818859</c:v>
-                  </c:pt>
-                  <c:pt idx="24">
-                    <c:v>37.027342540917701</c:v>
-                  </c:pt>
-                  <c:pt idx="25">
-                    <c:v>333.42559606679862</c:v>
-                  </c:pt>
-                  <c:pt idx="26">
-                    <c:v>87.362936749580342</c:v>
-                  </c:pt>
-                  <c:pt idx="27">
-                    <c:v>177.02776770143288</c:v>
-                  </c:pt>
-                  <c:pt idx="28">
-                    <c:v>199.81879506643384</c:v>
-                  </c:pt>
-                  <c:pt idx="29">
-                    <c:v>379.22121118685305</c:v>
-                  </c:pt>
-                  <c:pt idx="30">
-                    <c:v>144.76850275459859</c:v>
-                  </c:pt>
-                  <c:pt idx="31">
                     <c:v>1230.3773463183302</c:v>
-                  </c:pt>
-                  <c:pt idx="32">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="33">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="34">
-                    <c:v>0</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -10864,228 +10731,126 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>'Particles 5x E_CC'!$D$2:$D$36</c:f>
+              <c:f>('Particles 5x E_CC'!$D$2,'Particles 5x E_CC'!$D$17:$D$33)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="35"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9392547244381438E-2</c:v>
+                  <c:v>0.65934660630896891</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.8177641733144318E-2</c:v>
+                  <c:v>0.67873915355335046</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.11635528346628864</c:v>
+                  <c:v>0.69813170079773179</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.17453292519943295</c:v>
+                  <c:v>0.71752424804211334</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.23271056693257727</c:v>
+                  <c:v>0.73691679528649467</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.29088820866572157</c:v>
+                  <c:v>0.75630934253087612</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.3490658503988659</c:v>
+                  <c:v>0.77570188977525756</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.40724349213201022</c:v>
+                  <c:v>0.795094437019639</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.46542113386515455</c:v>
+                  <c:v>0.81448698426402044</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.52359877559829893</c:v>
+                  <c:v>0.83387953150840188</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.58177641733144314</c:v>
+                  <c:v>0.85327207875278333</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.60116896457582458</c:v>
+                  <c:v>0.87266462599716477</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.62056151182020602</c:v>
+                  <c:v>0.8920571732415461</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.63995405906458758</c:v>
+                  <c:v>0.91144972048592765</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.65934660630896891</c:v>
+                  <c:v>0.93084226773030909</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.67873915355335046</c:v>
+                  <c:v>0.95023481497469053</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.69813170079773179</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.71752424804211334</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.73691679528649467</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.75630934253087612</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.77570188977525756</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.795094437019639</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.81448698426402044</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.83387953150840188</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.85327207875278333</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.87266462599716477</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0.8920571732415461</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0.91144972048592765</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.93084226773030909</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.95023481497469053</c:v>
-                </c:pt>
-                <c:pt idx="31">
                   <c:v>0.96962736221907198</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0.98901990946345342</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>1.008412456707835</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>1.0278050039522162</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Particles 5x E_CC'!$L$2:$L$36</c:f>
+              <c:f>('Particles 5x E_CC'!$L$2,'Particles 5x E_CC'!$L$17:$L$33)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="35"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>123.30777734031922</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>112.07125821496713</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>156.76021003058847</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>209.13879130197765</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>126.50829446682214</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>195.82713362003696</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>195.65497516581365</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>267.69763999515436</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>211.6989006329689</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>548.21637163451351</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>459.28403343529482</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>456.87350843453771</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>764.51434401405254</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>998.56239210757451</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>123.30777734031922</c:v>
+                  <c:v>1050.4510811956754</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>112.07125821496713</c:v>
+                  <c:v>1310.6350888882159</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>156.76021003058847</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>209.13879130197765</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>126.50829446682214</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>195.82713362003696</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>195.65497516581365</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>267.69763999515436</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>211.6989006329689</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>548.21637163451351</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>459.28403343529482</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>456.87350843453771</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>764.51434401405254</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>998.56239210757451</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>1050.4510811956754</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>1310.6350888882159</c:v>
-                </c:pt>
-                <c:pt idx="31">
                   <c:v>2170.1321701141765</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11101,15 +10866,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Particles!$L$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>V_norm_1k</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Epsilon = 110</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -11133,6 +10890,253 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Particles!$M$2:$M$36</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="35"/>
+                  <c:pt idx="0">
+                    <c:v>3.8806091660975088E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.4358386186555265E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.12940978119910423</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.16239628557944297</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.34290391343640281</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.99361753942349473</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.65849904450955754</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0.34214892390595053</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>1.8179625909297472</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>3.0642519286360987</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>1.2138860600237567</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>2.1793366439035511</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>2.7824705108733863</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>2.703713958803704</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>16.44054328146337</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>4.489228504490498</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>5.058269646794245</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>3.6344620703578672</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>8.6481625542642941</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>10.225596658037613</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>7.3601653267253475</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
+                    <c:v>8.0023376222107743</c:v>
+                  </c:pt>
+                  <c:pt idx="22">
+                    <c:v>11.622344418619983</c:v>
+                  </c:pt>
+                  <c:pt idx="23">
+                    <c:v>12.509331983128806</c:v>
+                  </c:pt>
+                  <c:pt idx="24">
+                    <c:v>42.899465949910301</c:v>
+                  </c:pt>
+                  <c:pt idx="25">
+                    <c:v>11.478021702511715</c:v>
+                  </c:pt>
+                  <c:pt idx="26">
+                    <c:v>42.146960684955395</c:v>
+                  </c:pt>
+                  <c:pt idx="27">
+                    <c:v>38.789075272108697</c:v>
+                  </c:pt>
+                  <c:pt idx="28">
+                    <c:v>55.049759397228513</c:v>
+                  </c:pt>
+                  <c:pt idx="29">
+                    <c:v>51.456606458788386</c:v>
+                  </c:pt>
+                  <c:pt idx="30">
+                    <c:v>87.481507104921022</c:v>
+                  </c:pt>
+                  <c:pt idx="31">
+                    <c:v>93.166021490638045</c:v>
+                  </c:pt>
+                  <c:pt idx="32">
+                    <c:v>225.60366965697494</c:v>
+                  </c:pt>
+                  <c:pt idx="33">
+                    <c:v>92.532284629014327</c:v>
+                  </c:pt>
+                  <c:pt idx="34">
+                    <c:v>129.28020612941248</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Particles!$M$2:$M$36</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="35"/>
+                  <c:pt idx="0">
+                    <c:v>3.8806091660975088E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.4358386186555265E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.12940978119910423</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.16239628557944297</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.34290391343640281</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.99361753942349473</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.65849904450955754</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0.34214892390595053</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>1.8179625909297472</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>3.0642519286360987</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>1.2138860600237567</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>2.1793366439035511</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>2.7824705108733863</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>2.703713958803704</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>16.44054328146337</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>4.489228504490498</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>5.058269646794245</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>3.6344620703578672</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>8.6481625542642941</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>10.225596658037613</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>7.3601653267253475</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
+                    <c:v>8.0023376222107743</c:v>
+                  </c:pt>
+                  <c:pt idx="22">
+                    <c:v>11.622344418619983</c:v>
+                  </c:pt>
+                  <c:pt idx="23">
+                    <c:v>12.509331983128806</c:v>
+                  </c:pt>
+                  <c:pt idx="24">
+                    <c:v>42.899465949910301</c:v>
+                  </c:pt>
+                  <c:pt idx="25">
+                    <c:v>11.478021702511715</c:v>
+                  </c:pt>
+                  <c:pt idx="26">
+                    <c:v>42.146960684955395</c:v>
+                  </c:pt>
+                  <c:pt idx="27">
+                    <c:v>38.789075272108697</c:v>
+                  </c:pt>
+                  <c:pt idx="28">
+                    <c:v>55.049759397228513</c:v>
+                  </c:pt>
+                  <c:pt idx="29">
+                    <c:v>51.456606458788386</c:v>
+                  </c:pt>
+                  <c:pt idx="30">
+                    <c:v>87.481507104921022</c:v>
+                  </c:pt>
+                  <c:pt idx="31">
+                    <c:v>93.166021490638045</c:v>
+                  </c:pt>
+                  <c:pt idx="32">
+                    <c:v>225.60366965697494</c:v>
+                  </c:pt>
+                  <c:pt idx="33">
+                    <c:v>92.532284629014327</c:v>
+                  </c:pt>
+                  <c:pt idx="34">
+                    <c:v>129.28020612941248</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>Particles!$D$2:$D$36</c:f>
@@ -11445,6 +11449,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -11569,6 +11574,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -11647,6 +11653,47 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.17162311028548355"/>
+          <c:y val="0.18597149314668995"/>
+          <c:w val="0.17992426285038887"/>
+          <c:h val="0.15625109361329836"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -11755,6 +11802,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -13262,6 +13310,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14165,6 +14214,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -14288,6 +14338,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -14448,6 +14499,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14536,113 +14588,59 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>'Particles 10x Time'!$M$2:$M$36</c:f>
+                <c:f>('Particles 10x Time'!$M$2,'Particles 10x Time'!$M$13,'Particles 10x Time'!$M$16,'Particles 10x Time'!$M$19,'Particles 10x Time'!$M$22,'Particles 10x Time'!$M$25:$M$36)</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="35"/>
+                  <c:ptCount val="17"/>
                   <c:pt idx="0">
                     <c:v>3.5072496346851721E-3</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0</c:v>
+                    <c:v>16.286359155933233</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0</c:v>
+                    <c:v>17.177264202753584</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0</c:v>
+                    <c:v>2.837280101646642</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0</c:v>
+                    <c:v>0.92418149194300503</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0</c:v>
+                    <c:v>56.323593634852983</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0</c:v>
+                    <c:v>13.272401353939298</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>0</c:v>
+                    <c:v>31.787561084172527</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>0</c:v>
+                    <c:v>91.19302305628446</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>0</c:v>
+                    <c:v>2.9339698829060725</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>0</c:v>
+                    <c:v>4.4453328459464148</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>16.286359155933233</c:v>
+                    <c:v>34.248052266396101</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>0</c:v>
+                    <c:v>111.41419810428251</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>0</c:v>
+                    <c:v>77.068141050150587</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>17.177264202753584</c:v>
+                    <c:v>56.547463641776631</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>0</c:v>
+                    <c:v>174.49703253156585</c:v>
                   </c:pt>
                   <c:pt idx="16">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>2.837280101646642</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>0.92418149194300503</c:v>
-                  </c:pt>
-                  <c:pt idx="21">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="22">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="23">
-                    <c:v>56.323593634852983</c:v>
-                  </c:pt>
-                  <c:pt idx="24">
-                    <c:v>13.272401353939298</c:v>
-                  </c:pt>
-                  <c:pt idx="25">
-                    <c:v>31.787561084172527</c:v>
-                  </c:pt>
-                  <c:pt idx="26">
-                    <c:v>91.19302305628446</c:v>
-                  </c:pt>
-                  <c:pt idx="27">
-                    <c:v>2.9339698829060725</c:v>
-                  </c:pt>
-                  <c:pt idx="28">
-                    <c:v>4.4453328459464148</c:v>
-                  </c:pt>
-                  <c:pt idx="29">
-                    <c:v>34.248052266396101</c:v>
-                  </c:pt>
-                  <c:pt idx="30">
-                    <c:v>111.41419810428251</c:v>
-                  </c:pt>
-                  <c:pt idx="31">
-                    <c:v>77.068141050150587</c:v>
-                  </c:pt>
-                  <c:pt idx="32">
-                    <c:v>56.547463641776631</c:v>
-                  </c:pt>
-                  <c:pt idx="33">
-                    <c:v>174.49703253156585</c:v>
-                  </c:pt>
-                  <c:pt idx="34">
                     <c:v>536.81123572743616</c:v>
                   </c:pt>
                 </c:numCache>
@@ -14650,113 +14648,59 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>'Particles 10x Time'!$M$2:$M$36</c:f>
+                <c:f>('Particles 10x Time'!$M$2,'Particles 10x Time'!$M$13,'Particles 10x Time'!$M$16,'Particles 10x Time'!$M$19,'Particles 10x Time'!$M$22,'Particles 10x Time'!$M$25:$M$36)</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="35"/>
+                  <c:ptCount val="17"/>
                   <c:pt idx="0">
                     <c:v>3.5072496346851721E-3</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0</c:v>
+                    <c:v>16.286359155933233</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0</c:v>
+                    <c:v>17.177264202753584</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0</c:v>
+                    <c:v>2.837280101646642</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0</c:v>
+                    <c:v>0.92418149194300503</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0</c:v>
+                    <c:v>56.323593634852983</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0</c:v>
+                    <c:v>13.272401353939298</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>0</c:v>
+                    <c:v>31.787561084172527</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>0</c:v>
+                    <c:v>91.19302305628446</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>0</c:v>
+                    <c:v>2.9339698829060725</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>0</c:v>
+                    <c:v>4.4453328459464148</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>16.286359155933233</c:v>
+                    <c:v>34.248052266396101</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>0</c:v>
+                    <c:v>111.41419810428251</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>0</c:v>
+                    <c:v>77.068141050150587</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>17.177264202753584</c:v>
+                    <c:v>56.547463641776631</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>0</c:v>
+                    <c:v>174.49703253156585</c:v>
                   </c:pt>
                   <c:pt idx="16">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>2.837280101646642</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>0.92418149194300503</c:v>
-                  </c:pt>
-                  <c:pt idx="21">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="22">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="23">
-                    <c:v>56.323593634852983</c:v>
-                  </c:pt>
-                  <c:pt idx="24">
-                    <c:v>13.272401353939298</c:v>
-                  </c:pt>
-                  <c:pt idx="25">
-                    <c:v>31.787561084172527</c:v>
-                  </c:pt>
-                  <c:pt idx="26">
-                    <c:v>91.19302305628446</c:v>
-                  </c:pt>
-                  <c:pt idx="27">
-                    <c:v>2.9339698829060725</c:v>
-                  </c:pt>
-                  <c:pt idx="28">
-                    <c:v>4.4453328459464148</c:v>
-                  </c:pt>
-                  <c:pt idx="29">
-                    <c:v>34.248052266396101</c:v>
-                  </c:pt>
-                  <c:pt idx="30">
-                    <c:v>111.41419810428251</c:v>
-                  </c:pt>
-                  <c:pt idx="31">
-                    <c:v>77.068141050150587</c:v>
-                  </c:pt>
-                  <c:pt idx="32">
-                    <c:v>56.547463641776631</c:v>
-                  </c:pt>
-                  <c:pt idx="33">
-                    <c:v>174.49703253156585</c:v>
-                  </c:pt>
-                  <c:pt idx="34">
                     <c:v>536.81123572743616</c:v>
                   </c:pt>
                 </c:numCache>
@@ -14778,113 +14722,59 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>'Particles 10x Time'!$D$2:$D$36</c:f>
+              <c:f>('Particles 10x Time'!$D$2,'Particles 10x Time'!$D$13,'Particles 10x Time'!$D$16,'Particles 10x Time'!$D$19,'Particles 10x Time'!$D$22,'Particles 10x Time'!$D$25:$D$36)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="35"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9392547244381438E-2</c:v>
+                  <c:v>0.58177641733144314</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.8177641733144318E-2</c:v>
+                  <c:v>0.63995405906458758</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.11635528346628864</c:v>
+                  <c:v>0.69813170079773179</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.17453292519943295</c:v>
+                  <c:v>0.75630934253087612</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.23271056693257727</c:v>
+                  <c:v>0.81448698426402044</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.29088820866572157</c:v>
+                  <c:v>0.83387953150840188</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.3490658503988659</c:v>
+                  <c:v>0.85327207875278333</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.40724349213201022</c:v>
+                  <c:v>0.87266462599716477</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.46542113386515455</c:v>
+                  <c:v>0.8920571732415461</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.52359877559829893</c:v>
+                  <c:v>0.91144972048592765</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.58177641733144314</c:v>
+                  <c:v>0.93084226773030909</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.60116896457582458</c:v>
+                  <c:v>0.95023481497469053</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.62056151182020602</c:v>
+                  <c:v>0.96962736221907198</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.63995405906458758</c:v>
+                  <c:v>0.98901990946345342</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.65934660630896891</c:v>
+                  <c:v>1.008412456707835</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.67873915355335046</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.69813170079773179</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.71752424804211334</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.73691679528649467</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.75630934253087612</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.77570188977525756</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.795094437019639</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.81448698426402044</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.83387953150840188</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.85327207875278333</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.87266462599716477</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0.8920571732415461</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0.91144972048592765</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.93084226773030909</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.95023481497469053</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.96962736221907198</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0.98901990946345342</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>1.008412456707835</c:v>
-                </c:pt>
-                <c:pt idx="34">
                   <c:v>1.0278050039522162</c:v>
                 </c:pt>
               </c:numCache>
@@ -14892,114 +14782,60 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Particles 10x Time'!$L$2:$L$36</c:f>
+              <c:f>('Particles 10x Time'!$K$2,'Particles 10x Time'!$K$13,'Particles 10x Time'!$K$16,'Particles 10x Time'!$K$19,'Particles 10x Time'!$K$22,'Particles 10x Time'!$K$25:$K$36)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="35"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.3922400000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>60.323855000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>70.834130000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>89.544899999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>98.395125000000007</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>186.860885</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>187.71418499999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>237.57972000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>237.80999500000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>296.16845999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>385.39530500000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43.32863227604436</c:v>
+                  <c:v>370.61942999999997</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>705.41806500000007</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>967.26121999999998</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>50.877815606504619</c:v>
+                  <c:v>775.99524499999995</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>1192.941055</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>64.317143595931725</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>70.67396785037063</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>134.21600083318967</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>134.82889803482155</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>170.64566454059644</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>170.81106346606907</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>212.72802103085672</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>276.81671622708728</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>266.20369332873639</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>506.67849293225305</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>694.75178130207428</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>557.37174984198123</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>856.85015155432961</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>948.30025354823863</c:v>
+                  <c:v>1320.2615449999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15345,6 +15181,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -15467,6 +15304,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -31413,8 +31251,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T60"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AE10" sqref="AE10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33201,7 +33039,7 @@
   <dimension ref="A1:T81"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="AE11" sqref="AE11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34673,130 +34511,90 @@
       <c r="D40">
         <v>1.9392547244381438E-2</v>
       </c>
-      <c r="E40" t="e">
-        <f t="shared" ref="E40:E73" si="6">L3</f>
-        <v>#DIV/0!</v>
-      </c>
       <c r="F40">
-        <f t="shared" ref="F40:F81" si="7">(1-D40/$J$58)^(-2)*(1-$J$59*D40/$J$58+$J$60*(D40/$J$58)^2)</f>
-        <v>1.0368774959931355</v>
+        <f t="shared" ref="F40:F81" si="6">(1-D40/$J$58)^(-2)*(1-$J$59*D40/$J$58+$J$60*(D40/$J$58)^2)</f>
+        <v>1.0301893897675021</v>
       </c>
     </row>
     <row r="41" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D41">
         <v>5.8177641733144318E-2</v>
       </c>
-      <c r="E41" t="e">
+      <c r="F41">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F41">
-        <f t="shared" si="7"/>
-        <v>1.1742415121718948</v>
+        <v>1.0962416171645919</v>
       </c>
     </row>
     <row r="42" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D42">
         <v>0.11635528346628864</v>
       </c>
-      <c r="E42" t="e">
+      <c r="F42">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F42">
-        <f t="shared" si="7"/>
-        <v>1.5680794373436795</v>
+        <v>1.2119640307752102</v>
       </c>
     </row>
     <row r="43" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D43">
         <v>0.17453292519943295</v>
       </c>
-      <c r="E43" t="e">
+      <c r="F43">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F43">
-        <f t="shared" si="7"/>
-        <v>2.2432919345776541</v>
+        <v>1.3526120008408742</v>
       </c>
     </row>
     <row r="44" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D44">
         <v>0.23271056693257727</v>
       </c>
-      <c r="E44" t="e">
+      <c r="F44">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F44">
-        <f t="shared" si="7"/>
-        <v>3.2803791987232569</v>
+        <v>1.525646867927472</v>
       </c>
     </row>
     <row r="45" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D45">
         <v>0.29088820866572157</v>
       </c>
-      <c r="E45" t="e">
+      <c r="F45">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F45">
-        <f t="shared" si="7"/>
-        <v>4.785248297621723</v>
+        <v>1.7415073549536146</v>
       </c>
     </row>
     <row r="46" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D46">
         <v>0.3490658503988659</v>
       </c>
-      <c r="E46" t="e">
+      <c r="F46">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F46">
-        <f t="shared" si="7"/>
-        <v>6.8987427786497859</v>
+        <v>2.0151478038015225</v>
       </c>
     </row>
     <row r="47" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D47">
         <v>0.40724349213201022</v>
       </c>
-      <c r="E47" t="e">
+      <c r="F47">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F47">
-        <f t="shared" si="7"/>
-        <v>9.8104562528729033</v>
+        <v>2.3685862490418956</v>
       </c>
     </row>
     <row r="48" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D48">
         <v>0.46542113386515455</v>
       </c>
-      <c r="E48" t="e">
+      <c r="F48">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F48">
-        <f t="shared" si="7"/>
-        <v>13.779130521396597</v>
+        <v>2.8352955296716074</v>
       </c>
     </row>
     <row r="49" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D49">
         <v>0.52359877559829893</v>
       </c>
-      <c r="E49" t="e">
+      <c r="F49">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F49">
-        <f t="shared" si="7"/>
-        <v>19.163407336613755</v>
+        <v>3.4681304939327204</v>
       </c>
     </row>
     <row r="50" spans="4:10" x14ac:dyDescent="0.25">
@@ -34804,38 +34602,30 @@
         <v>0.58177641733144314</v>
       </c>
       <c r="E50">
+        <f t="shared" ref="E40:E73" si="7">L13</f>
+        <v>43.32863227604436</v>
+      </c>
+      <c r="F50">
         <f t="shared" si="6"/>
-        <v>43.32863227604436</v>
-      </c>
-      <c r="F50">
-        <f t="shared" si="7"/>
-        <v>26.469281139594774</v>
+        <v>4.3544548615869676</v>
       </c>
     </row>
     <row r="51" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D51">
         <v>0.60116896457582458</v>
       </c>
-      <c r="E51" t="e">
+      <c r="F51">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F51">
-        <f t="shared" si="7"/>
-        <v>29.449093448705653</v>
+        <v>4.7297584036803864</v>
       </c>
     </row>
     <row r="52" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D52">
         <v>0.62056151182020602</v>
       </c>
-      <c r="E52" t="e">
+      <c r="F52">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F52">
-        <f t="shared" si="7"/>
-        <v>32.754773407760844</v>
+        <v>5.1572740816545934</v>
       </c>
     </row>
     <row r="53" spans="4:10" x14ac:dyDescent="0.25">
@@ -34843,38 +34633,30 @@
         <v>0.63995405906458758</v>
       </c>
       <c r="E53">
+        <f t="shared" si="7"/>
+        <v>50.877815606504619</v>
+      </c>
+      <c r="F53">
         <f t="shared" si="6"/>
-        <v>50.877815606504619</v>
-      </c>
-      <c r="F53">
-        <f t="shared" si="7"/>
-        <v>36.425278318672731</v>
+        <v>5.6470195462680248</v>
       </c>
     </row>
     <row r="54" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D54">
         <v>0.65934660630896891</v>
       </c>
-      <c r="E54" t="e">
+      <c r="F54">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F54">
-        <f t="shared" si="7"/>
-        <v>40.505159797121827</v>
+        <v>6.2115218420437621</v>
       </c>
     </row>
     <row r="55" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D55">
         <v>0.67873915355335046</v>
       </c>
-      <c r="E55" t="e">
+      <c r="F55">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F55">
-        <f t="shared" si="7"/>
-        <v>45.045526038285914</v>
+        <v>6.8666091366086244</v>
       </c>
     </row>
     <row r="56" spans="4:10" x14ac:dyDescent="0.25">
@@ -34882,51 +34664,43 @@
         <v>0.69813170079773179</v>
       </c>
       <c r="E56">
+        <f t="shared" si="7"/>
+        <v>64.317143595931725</v>
+      </c>
+      <c r="F56">
         <f t="shared" si="6"/>
-        <v>64.317143595931725</v>
-      </c>
-      <c r="F56">
-        <f t="shared" si="7"/>
-        <v>50.105199617956551</v>
+        <v>7.632509479469844</v>
       </c>
     </row>
     <row r="57" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D57">
         <v>0.71752424804211334</v>
       </c>
-      <c r="E57" t="e">
+      <c r="F57">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F57">
-        <f t="shared" si="7"/>
-        <v>55.752117131314037</v>
+        <v>8.5354004548607314</v>
       </c>
       <c r="I57" t="s">
         <v>32</v>
       </c>
-      <c r="J57" t="e">
+      <c r="J57">
         <f>SUMXMY2(E39:E73,F39:F73)</f>
-        <v>#DIV/0!</v>
+        <v>1037389.7831871572</v>
       </c>
     </row>
     <row r="58" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D58">
         <v>0.73691679528649467</v>
       </c>
-      <c r="E58" t="e">
+      <c r="F58">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F58">
-        <f t="shared" si="7"/>
-        <v>62.065029599807239</v>
+        <v>9.6096340654112424</v>
       </c>
       <c r="I58" t="s">
         <v>33</v>
       </c>
       <c r="J58">
-        <v>1.3980065201780481</v>
+        <v>1.0584547729979594</v>
       </c>
     </row>
     <row r="59" spans="4:10" x14ac:dyDescent="0.25">
@@ -34934,50 +34708,42 @@
         <v>0.75630934253087612</v>
       </c>
       <c r="E59">
+        <f t="shared" si="7"/>
+        <v>70.67396785037063</v>
+      </c>
+      <c r="F59">
         <f t="shared" si="6"/>
-        <v>70.67396785037063</v>
-      </c>
-      <c r="F59">
-        <f t="shared" si="7"/>
-        <v>69.135579133252619</v>
+        <v>10.90099493757957</v>
       </c>
       <c r="I59" t="s">
         <v>34</v>
       </c>
       <c r="J59">
-        <v>4.501589282315735E-2</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="60" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D60">
         <v>0.77570188977525756</v>
       </c>
-      <c r="E60" t="e">
+      <c r="F60">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F60">
-        <f t="shared" si="7"/>
-        <v>77.070849202300593</v>
+        <v>12.471578501343851</v>
       </c>
       <c r="I60" t="s">
         <v>35</v>
       </c>
       <c r="J60">
-        <v>46.435871274294229</v>
+        <v>0.34100000000000003</v>
       </c>
     </row>
     <row r="61" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D61">
         <v>0.795094437019639</v>
       </c>
-      <c r="E61" t="e">
+      <c r="F61">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F61">
-        <f t="shared" si="7"/>
-        <v>85.996514985951606</v>
+        <v>14.407278658280561</v>
       </c>
     </row>
     <row r="62" spans="4:10" x14ac:dyDescent="0.25">
@@ -34985,12 +34751,12 @@
         <v>0.81448698426402044</v>
       </c>
       <c r="E62">
+        <f t="shared" si="7"/>
+        <v>134.21600083318967</v>
+      </c>
+      <c r="F62">
         <f t="shared" si="6"/>
-        <v>134.21600083318967</v>
-      </c>
-      <c r="F62">
-        <f t="shared" si="7"/>
-        <v>96.060759329278596</v>
+        <v>16.829609750345881</v>
       </c>
     </row>
     <row r="63" spans="4:10" x14ac:dyDescent="0.25">
@@ -34998,12 +34764,12 @@
         <v>0.83387953150840188</v>
       </c>
       <c r="E63">
+        <f t="shared" si="7"/>
+        <v>134.82889803482155</v>
+      </c>
+      <c r="F63">
         <f t="shared" si="6"/>
-        <v>134.82889803482155</v>
-      </c>
-      <c r="F63">
-        <f t="shared" si="7"/>
-        <v>107.43917274810902</v>
+        <v>19.914983935992684</v>
       </c>
     </row>
     <row r="64" spans="4:10" x14ac:dyDescent="0.25">
@@ -35011,12 +34777,12 @@
         <v>0.85327207875278333</v>
       </c>
       <c r="E64">
+        <f t="shared" si="7"/>
+        <v>170.64566454059644</v>
+      </c>
+      <c r="F64">
         <f t="shared" si="6"/>
-        <v>170.64566454059644</v>
-      </c>
-      <c r="F64">
-        <f t="shared" si="7"/>
-        <v>120.34092821668052</v>
+        <v>23.927339732875247</v>
       </c>
     </row>
     <row r="65" spans="4:6" x14ac:dyDescent="0.25">
@@ -35024,12 +34790,12 @@
         <v>0.87266462599716477</v>
       </c>
       <c r="E65">
+        <f t="shared" si="7"/>
+        <v>170.81106346606907</v>
+      </c>
+      <c r="F65">
         <f t="shared" si="6"/>
-        <v>170.81106346606907</v>
-      </c>
-      <c r="F65">
-        <f t="shared" si="7"/>
-        <v>135.01662126874359</v>
+        <v>29.275828968053169</v>
       </c>
     </row>
     <row r="66" spans="4:6" x14ac:dyDescent="0.25">
@@ -35037,12 +34803,12 @@
         <v>0.8920571732415461</v>
       </c>
       <c r="E66">
+        <f t="shared" si="7"/>
+        <v>212.72802103085672</v>
+      </c>
+      <c r="F66">
         <f t="shared" si="6"/>
-        <v>212.72802103085672</v>
-      </c>
-      <c r="F66">
-        <f t="shared" si="7"/>
-        <v>151.76830515398774</v>
+        <v>36.622216837623625</v>
       </c>
     </row>
     <row r="67" spans="4:6" x14ac:dyDescent="0.25">
@@ -35050,12 +34816,12 @@
         <v>0.91144972048592765</v>
       </c>
       <c r="E67">
+        <f t="shared" si="7"/>
+        <v>276.81671622708728</v>
+      </c>
+      <c r="F67">
         <f t="shared" si="6"/>
-        <v>276.81671622708728</v>
-      </c>
-      <c r="F67">
-        <f t="shared" si="7"/>
-        <v>170.96244719918877</v>
+        <v>47.093700304889502</v>
       </c>
     </row>
     <row r="68" spans="4:6" x14ac:dyDescent="0.25">
@@ -35063,12 +34829,12 @@
         <v>0.93084226773030909</v>
       </c>
       <c r="E68">
+        <f t="shared" si="7"/>
+        <v>266.20369332873639</v>
+      </c>
+      <c r="F68">
         <f t="shared" si="6"/>
-        <v>266.20369332873639</v>
-      </c>
-      <c r="F68">
-        <f t="shared" si="7"/>
-        <v>193.04681300848333</v>
+        <v>62.738294836510747</v>
       </c>
     </row>
     <row r="69" spans="4:6" x14ac:dyDescent="0.25">
@@ -35076,12 +34842,12 @@
         <v>0.95023481497469053</v>
       </c>
       <c r="E69">
+        <f t="shared" si="7"/>
+        <v>506.67849293225305</v>
+      </c>
+      <c r="F69">
         <f t="shared" si="6"/>
-        <v>506.67849293225305</v>
-      </c>
-      <c r="F69">
-        <f t="shared" si="7"/>
-        <v>218.57269094736108</v>
+        <v>87.598833272317279</v>
       </c>
     </row>
     <row r="70" spans="4:6" x14ac:dyDescent="0.25">
@@ -35089,12 +34855,12 @@
         <v>0.96962736221907198</v>
       </c>
       <c r="E70">
+        <f t="shared" si="7"/>
+        <v>694.75178130207428</v>
+      </c>
+      <c r="F70">
         <f t="shared" si="6"/>
-        <v>694.75178130207428</v>
-      </c>
-      <c r="F70">
-        <f t="shared" si="7"/>
-        <v>248.22446479430565</v>
+        <v>130.59111722045046</v>
       </c>
     </row>
     <row r="71" spans="4:6" x14ac:dyDescent="0.25">
@@ -35102,12 +34868,12 @@
         <v>0.98901990946345342</v>
       </c>
       <c r="E71">
+        <f t="shared" si="7"/>
+        <v>557.37174984198123</v>
+      </c>
+      <c r="F71">
         <f t="shared" si="6"/>
-        <v>557.37174984198123</v>
-      </c>
-      <c r="F71">
-        <f t="shared" si="7"/>
-        <v>282.85942949143924</v>
+        <v>214.70712689046451</v>
       </c>
     </row>
     <row r="72" spans="4:6" x14ac:dyDescent="0.25">
@@ -35115,12 +34881,12 @@
         <v>1.008412456707835</v>
       </c>
       <c r="E72">
+        <f t="shared" si="7"/>
+        <v>856.85015155432961</v>
+      </c>
+      <c r="F72">
         <f t="shared" si="6"/>
-        <v>856.85015155432961</v>
-      </c>
-      <c r="F72">
-        <f t="shared" si="7"/>
-        <v>323.56208833184695</v>
+        <v>415.35438948145787</v>
       </c>
     </row>
     <row r="73" spans="4:6" x14ac:dyDescent="0.25">
@@ -35128,12 +34894,12 @@
         <v>1.0278050039522162</v>
       </c>
       <c r="E73">
+        <f t="shared" si="7"/>
+        <v>948.30025354823863</v>
+      </c>
+      <c r="F73">
         <f t="shared" si="6"/>
-        <v>948.30025354823863</v>
-      </c>
-      <c r="F73">
-        <f t="shared" si="7"/>
-        <v>371.71924125522042</v>
+        <v>1112.8271490493012</v>
       </c>
     </row>
     <row r="74" spans="4:6" x14ac:dyDescent="0.25">
@@ -35141,8 +34907,8 @@
         <v>1.0471975511966001</v>
       </c>
       <c r="F74">
-        <f t="shared" si="7"/>
-        <v>429.12543074971887</v>
+        <f t="shared" si="6"/>
+        <v>8292.8388123746554</v>
       </c>
     </row>
     <row r="75" spans="4:6" x14ac:dyDescent="0.25">
@@ -35150,8 +34916,8 @@
         <v>1.06659009844098</v>
       </c>
       <c r="F75">
-        <f t="shared" si="7"/>
-        <v>498.13354384328193</v>
+        <f t="shared" si="6"/>
+        <v>15965.879068402734</v>
       </c>
     </row>
     <row r="76" spans="4:6" x14ac:dyDescent="0.25">
@@ -35159,8 +34925,8 @@
         <v>1.0859826456853601</v>
       </c>
       <c r="F76">
-        <f t="shared" si="7"/>
-        <v>581.8739750427128</v>
+        <f t="shared" si="6"/>
+        <v>1402.381944135788</v>
       </c>
     </row>
     <row r="77" spans="4:6" x14ac:dyDescent="0.25">
@@ -35168,8 +34934,8 @@
         <v>1.10537519292974</v>
       </c>
       <c r="F77">
-        <f t="shared" si="7"/>
-        <v>684.58028848384151</v>
+        <f t="shared" si="6"/>
+        <v>485.56458701142759</v>
       </c>
     </row>
     <row r="78" spans="4:6" x14ac:dyDescent="0.25">
@@ -35177,8 +34943,8 @@
         <v>1.1247677401741201</v>
       </c>
       <c r="F78">
-        <f t="shared" si="7"/>
-        <v>812.08458807055774</v>
+        <f t="shared" si="6"/>
+        <v>244.58038465276991</v>
       </c>
     </row>
     <row r="79" spans="4:6" x14ac:dyDescent="0.25">
@@ -35186,8 +34952,8 @@
         <v>1.1441602874185</v>
       </c>
       <c r="F79">
-        <f t="shared" si="7"/>
-        <v>972.59121008359875</v>
+        <f t="shared" si="6"/>
+        <v>147.3450860398799</v>
       </c>
     </row>
     <row r="80" spans="4:6" x14ac:dyDescent="0.25">
@@ -35195,8 +34961,8 @@
         <v>1.1635528346628801</v>
       </c>
       <c r="F80">
-        <f t="shared" si="7"/>
-        <v>1177.9220202492395</v>
+        <f t="shared" si="6"/>
+        <v>98.624217400842184</v>
       </c>
     </row>
     <row r="81" spans="4:6" x14ac:dyDescent="0.25">
@@ -35204,8 +34970,8 @@
         <v>1.1829453819072699</v>
       </c>
       <c r="F81">
-        <f t="shared" si="7"/>
-        <v>1445.5912978904887</v>
+        <f t="shared" si="6"/>
+        <v>70.762470246647851</v>
       </c>
     </row>
   </sheetData>
@@ -35219,8 +34985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH100"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+    <sheetView topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35603,7 +35369,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>0.2</v>
+        <v>4.5</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
@@ -39944,7 +39710,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="R49" sqref="R49:R53"/>
     </sheetView>
   </sheetViews>
@@ -42228,19 +41994,19 @@
         <v>9.3338095116624192E-3</v>
       </c>
       <c r="Z39" s="10">
-        <f>E2</f>
+        <f t="shared" ref="Z39:Z68" si="22">E2</f>
         <v>0</v>
       </c>
       <c r="AA39">
-        <f>M2</f>
+        <f t="shared" ref="AA39:AA68" si="23">M2</f>
         <v>1</v>
       </c>
       <c r="AB39">
-        <f t="shared" ref="AB39:AB66" si="22">(1-Z39/$AG$52)^(-2)*(1-$AG$53*Z39/$AG$52+$AG$54*(Z39/$AG$52)^2)</f>
+        <f t="shared" ref="AB39:AB66" si="24">(1-Z39/$AG$52)^(-2)*(1-$AG$53*Z39/$AG$52+$AG$54*(Z39/$AG$52)^2)</f>
         <v>1</v>
       </c>
       <c r="AC39">
-        <f t="shared" ref="AC39:AC66" si="23">1+2.5*Z39+6.2*Z39^2</f>
+        <f t="shared" ref="AC39:AC66" si="25">1+2.5*Z39+6.2*Z39^2</f>
         <v>1</v>
       </c>
     </row>
@@ -42291,19 +42057,19 @@
         <v>1.2162236636408691E-2</v>
       </c>
       <c r="Z40" s="10">
-        <f>E3</f>
+        <f t="shared" si="22"/>
         <v>5.8177641733144318E-2</v>
       </c>
       <c r="AA40">
-        <f>M3</f>
+        <f t="shared" si="23"/>
         <v>1.7209360620221659</v>
       </c>
       <c r="AB40">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>1.0641542223008673</v>
       </c>
       <c r="AC40">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>1.1664288599181674</v>
       </c>
     </row>
@@ -42354,19 +42120,19 @@
         <v>2.8284271247458785E-4</v>
       </c>
       <c r="Z41" s="10">
-        <f>E4</f>
+        <f t="shared" si="22"/>
         <v>0.11635528346628864</v>
       </c>
       <c r="AA41">
-        <f>M4</f>
+        <f t="shared" si="23"/>
         <v>2.7538235662745518</v>
       </c>
       <c r="AB41">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>1.1406644568314936</v>
       </c>
       <c r="AC41">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>1.374827231006948</v>
       </c>
     </row>
@@ -42417,19 +42183,19 @@
         <v>3.1112698372208589E-3</v>
       </c>
       <c r="Z42" s="10">
-        <f>E5</f>
+        <f t="shared" si="22"/>
         <v>0.17453292519943295</v>
       </c>
       <c r="AA42">
-        <f>M5</f>
+        <f t="shared" si="23"/>
         <v>3.0934808687400404</v>
       </c>
       <c r="AB42">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>1.2330541399593167</v>
       </c>
       <c r="AC42">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>1.6251951132663416</v>
       </c>
     </row>
@@ -42480,19 +42246,19 @@
         <v>5.7275649276110323E-3</v>
       </c>
       <c r="Z43" s="10">
-        <f>E6</f>
+        <f t="shared" si="22"/>
         <v>0.23271056693257727</v>
       </c>
       <c r="AA43">
-        <f>M6</f>
+        <f t="shared" si="23"/>
         <v>4.3929132871389944</v>
       </c>
       <c r="AB43">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>1.3462220178267004</v>
       </c>
       <c r="AC43">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>1.9175325066963487</v>
       </c>
     </row>
@@ -42547,19 +42313,19 @@
         <v>5.6074355398286323E-3</v>
       </c>
       <c r="Z44" s="10">
-        <f>E7</f>
+        <f t="shared" si="22"/>
         <v>0.29088820866572157</v>
       </c>
       <c r="AA44">
-        <f>M7</f>
+        <f t="shared" si="23"/>
         <v>5.1153032174893909</v>
       </c>
       <c r="AB44">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>1.4871471140256687</v>
       </c>
       <c r="AC44">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>2.2518394112969689</v>
       </c>
     </row>
@@ -42614,19 +42380,19 @@
         <v>8.8831300789755478E-3</v>
       </c>
       <c r="Z45" s="10">
-        <f>E8</f>
+        <f t="shared" si="22"/>
         <v>0.3490658503988659</v>
       </c>
       <c r="AA45">
-        <f>M8</f>
+        <f t="shared" si="23"/>
         <v>5.9682202049500761</v>
       </c>
       <c r="AB45">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>1.6660570421975707</v>
       </c>
       <c r="AC45">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>2.6281158270682017</v>
       </c>
     </row>
@@ -42681,19 +42447,19 @@
         <v>1.8083141320025342E-3</v>
       </c>
       <c r="Z46" s="10">
-        <f>E9</f>
+        <f t="shared" si="22"/>
         <v>0.40724349213201022</v>
       </c>
       <c r="AA46">
-        <f>M9</f>
+        <f t="shared" si="23"/>
         <v>8.9541172047053745</v>
       </c>
       <c r="AB46">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>1.8984449645076611</v>
       </c>
       <c r="AC46">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>3.0463617540100483</v>
       </c>
     </row>
@@ -42748,19 +42514,19 @@
         <v>3.2908965343808891E-3</v>
       </c>
       <c r="Z47" s="10">
-        <f>E10</f>
+        <f t="shared" si="22"/>
         <v>0.46542113386515455</v>
       </c>
       <c r="AA47">
-        <f>M10</f>
+        <f t="shared" si="23"/>
         <v>8.7835753463083304</v>
       </c>
       <c r="AB47">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>2.2087234913616691</v>
       </c>
       <c r="AC47">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>3.5065771921225082</v>
       </c>
     </row>
@@ -42815,19 +42581,19 @@
         <v>6.4593601334291375E-3</v>
       </c>
       <c r="Z48" s="10">
-        <f>E11</f>
+        <f t="shared" si="22"/>
         <v>0.52359877559829893</v>
       </c>
       <c r="AA48">
-        <f>M11</f>
+        <f t="shared" si="23"/>
         <v>10.522671632259641</v>
       </c>
       <c r="AB48">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>2.6372371828549643</v>
       </c>
       <c r="AC48">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>4.0087621414055814</v>
       </c>
     </row>
@@ -42886,19 +42652,19 @@
         <v>3.0836936726378783E-3</v>
       </c>
       <c r="Z49" s="10">
-        <f>E12</f>
+        <f t="shared" si="22"/>
         <v>0.58177641733144314</v>
       </c>
       <c r="AA49">
-        <f>M12</f>
+        <f t="shared" si="23"/>
         <v>13.782105960502049</v>
       </c>
       <c r="AB49">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>3.2547032364445414</v>
       </c>
       <c r="AC49">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>4.5529166018592671</v>
       </c>
     </row>
@@ -42957,19 +42723,19 @@
         <v>5.3978390738023225E-3</v>
       </c>
       <c r="Z50" s="10">
-        <f>E13</f>
+        <f t="shared" si="22"/>
         <v>0.60116896457582458</v>
       </c>
       <c r="AA50">
-        <f>M13</f>
+        <f t="shared" si="23"/>
         <v>19.263832339617913</v>
       </c>
       <c r="AB50">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>3.5226798307383134</v>
       </c>
       <c r="AC50">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>4.7436279800484096</v>
       </c>
     </row>
@@ -43028,19 +42794,19 @@
         <v>4.2762912279996589E-3</v>
       </c>
       <c r="Z51" s="10">
-        <f>E14</f>
+        <f t="shared" si="22"/>
         <v>0.62056151182020602</v>
       </c>
       <c r="AA51">
-        <f>M14</f>
+        <f t="shared" si="23"/>
         <v>16.285260783155177</v>
       </c>
       <c r="AB51">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>3.8328396809773393</v>
       </c>
       <c r="AC51">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>4.9390026372565092</v>
       </c>
       <c r="AF51" t="s">
@@ -43106,19 +42872,19 @@
         <v>7.1625763521236275E-3</v>
       </c>
       <c r="Z52" s="10">
-        <f>E15</f>
+        <f t="shared" si="22"/>
         <v>0.63995405906458758</v>
       </c>
       <c r="AA52">
-        <f>M15</f>
+        <f t="shared" si="23"/>
         <v>29.005869187660018</v>
       </c>
       <c r="AB52">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>4.194690234058327</v>
       </c>
       <c r="AC52">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>5.1390405734835678</v>
       </c>
       <c r="AF52" t="s">
@@ -43183,19 +42949,19 @@
         <v>9.6586317181403814E-3</v>
       </c>
       <c r="Z53" s="10">
-        <f>E16</f>
+        <f t="shared" si="22"/>
         <v>0.65934660630896891</v>
       </c>
       <c r="AA53">
-        <f>M16</f>
+        <f t="shared" si="23"/>
         <v>19.930772949454798</v>
       </c>
       <c r="AB53">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>4.6205979240218911</v>
       </c>
       <c r="AC53">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>5.3437417887295799</v>
       </c>
       <c r="AF53" t="s">
@@ -43263,19 +43029,19 @@
         <v>6.7737237420294281E-3</v>
       </c>
       <c r="Z54" s="10">
-        <f>E17</f>
+        <f t="shared" si="22"/>
         <v>0.67873915355335046</v>
       </c>
       <c r="AA54">
-        <f>M17</f>
+        <f t="shared" si="23"/>
         <v>25.549671447243558</v>
       </c>
       <c r="AB54">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>5.1268898337224451</v>
       </c>
       <c r="AC54">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>5.5531062829945519</v>
       </c>
       <c r="AF54" t="s">
@@ -43343,19 +43109,19 @@
         <v>5.4464055424961787E-3</v>
       </c>
       <c r="Z55" s="10">
-        <f>E18</f>
+        <f t="shared" si="22"/>
         <v>0.69813170079773179</v>
       </c>
       <c r="AA55">
-        <f>M18</f>
+        <f t="shared" si="23"/>
         <v>33.32206943474602</v>
       </c>
       <c r="AB55">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>5.7354856552558662</v>
       </c>
       <c r="AC55">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>5.7671340562784783</v>
       </c>
     </row>
@@ -43414,19 +43180,19 @@
         <v>5.6794952827401088E-3</v>
       </c>
       <c r="Z56" s="10">
-        <f>E19</f>
+        <f t="shared" si="22"/>
         <v>0.71752424804211334</v>
       </c>
       <c r="AA56">
-        <f>M19</f>
+        <f t="shared" si="23"/>
         <v>32.845795061861018</v>
       </c>
       <c r="AB56">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>6.4763735735278996</v>
       </c>
       <c r="AC56">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>5.9858251085813645</v>
       </c>
     </row>
@@ -43485,19 +43251,19 @@
         <v>7.987229390303793E-3</v>
       </c>
       <c r="Z57" s="10">
-        <f>E20</f>
+        <f t="shared" si="22"/>
         <v>0.73691679528649467</v>
       </c>
       <c r="AA57">
-        <f>M20</f>
+        <f t="shared" si="23"/>
         <v>31.553218384630529</v>
       </c>
       <c r="AB57">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>7.3914691509128039</v>
       </c>
       <c r="AC57">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>6.2091794399032061</v>
       </c>
     </row>
@@ -43556,19 +43322,19 @@
         <v>6.88984760353959E-3</v>
       </c>
       <c r="Z58" s="10">
-        <f>E21</f>
+        <f t="shared" si="22"/>
         <v>0.75630934253087612</v>
       </c>
       <c r="AA58">
-        <f>M21</f>
+        <f t="shared" si="23"/>
         <v>38.422925283343176</v>
       </c>
       <c r="AB58">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>8.5408174950994713</v>
       </c>
       <c r="AC58">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>6.4371970502440039</v>
       </c>
     </row>
@@ -43598,11 +43364,11 @@
       </c>
       <c r="K59" s="3"/>
       <c r="L59">
-        <f t="shared" ref="L59:L68" si="24">AVERAGE(G59:K59)</f>
+        <f t="shared" ref="L59:L68" si="26">AVERAGE(G59:K59)</f>
         <v>1.0290750000000002</v>
       </c>
       <c r="N59">
-        <f t="shared" ref="N59:N68" si="25">_xlfn.STDEV.S(G59:K59)</f>
+        <f t="shared" ref="N59:N68" si="27">_xlfn.STDEV.S(G59:K59)</f>
         <v>4.4017988747026698E-3</v>
       </c>
       <c r="O59">
@@ -43619,27 +43385,27 @@
       </c>
       <c r="S59" s="3"/>
       <c r="T59">
-        <f t="shared" ref="T59:T68" si="26">AVERAGE(O59:S59)</f>
+        <f t="shared" ref="T59:T68" si="28">AVERAGE(O59:S59)</f>
         <v>1.0004999999999999</v>
       </c>
       <c r="U59">
-        <f t="shared" ref="U59:U68" si="27">_xlfn.STDEV.S(O59:S59)</f>
+        <f t="shared" ref="U59:U68" si="29">_xlfn.STDEV.S(O59:S59)</f>
         <v>8.8863190729720886E-3</v>
       </c>
       <c r="Z59" s="10">
-        <f>E22</f>
+        <f t="shared" si="22"/>
         <v>0.77570188977525756</v>
       </c>
       <c r="AA59">
-        <f>M22</f>
+        <f t="shared" si="23"/>
         <v>45.402014288016325</v>
       </c>
       <c r="AB59">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>10.012920660430149</v>
       </c>
       <c r="AC59">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>6.6698779396037597</v>
       </c>
     </row>
@@ -43669,11 +43435,11 @@
       </c>
       <c r="K60" s="3"/>
       <c r="L60">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>1.0307499999999998</v>
       </c>
       <c r="N60">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>3.8353617821530431E-3</v>
       </c>
       <c r="O60">
@@ -43690,27 +43456,27 @@
       </c>
       <c r="S60" s="3"/>
       <c r="T60">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>1.006375</v>
       </c>
       <c r="U60">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>1.8944194361334054E-2</v>
       </c>
       <c r="Z60" s="10">
-        <f>E23</f>
+        <f t="shared" si="22"/>
         <v>0.795094437019639</v>
       </c>
       <c r="AA60">
-        <f>M23</f>
+        <f t="shared" si="23"/>
         <v>52.493142468353298</v>
       </c>
       <c r="AB60">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>11.942657069256455</v>
       </c>
       <c r="AC60">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>6.9072221079824736</v>
       </c>
     </row>
@@ -43740,11 +43506,11 @@
       </c>
       <c r="K61" s="3"/>
       <c r="L61">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>1.0318749999999999</v>
       </c>
       <c r="N61">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>4.9358383279843997E-3</v>
       </c>
       <c r="O61">
@@ -43761,27 +43527,27 @@
       </c>
       <c r="S61" s="3"/>
       <c r="T61">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>0.99907499999999994</v>
       </c>
       <c r="U61">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>4.8403684432764636E-3</v>
       </c>
       <c r="Z61" s="10">
-        <f>E24</f>
+        <f t="shared" si="22"/>
         <v>0.81448698426402044</v>
       </c>
       <c r="AA61">
-        <f>M24</f>
+        <f t="shared" si="23"/>
         <v>84.594574850942678</v>
       </c>
       <c r="AB61">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>14.54392173907385</v>
       </c>
       <c r="AC61">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>7.1492295553801428</v>
       </c>
     </row>
@@ -43811,11 +43577,11 @@
       </c>
       <c r="K62" s="3"/>
       <c r="L62">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>1.0342</v>
       </c>
       <c r="N62">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>9.5439335007463065E-3</v>
       </c>
       <c r="O62">
@@ -43832,27 +43598,27 @@
       </c>
       <c r="S62" s="3"/>
       <c r="T62">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>1.0033999999999998</v>
       </c>
       <c r="U62">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>1.3620817400826834E-2</v>
       </c>
       <c r="Z62" s="10">
-        <f>E25</f>
+        <f t="shared" si="22"/>
         <v>0.83387953150840188</v>
       </c>
       <c r="AA62">
-        <f>M25</f>
+        <f t="shared" si="23"/>
         <v>103.11329788186424</v>
       </c>
       <c r="AB62">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>18.172644597879472</v>
       </c>
       <c r="AC62">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>7.3959002817967701</v>
       </c>
     </row>
@@ -43882,11 +43648,11 @@
       </c>
       <c r="K63" s="3"/>
       <c r="L63">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>1.0326250000000001</v>
       </c>
       <c r="N63">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>9.8048882366569383E-3</v>
       </c>
       <c r="O63">
@@ -43903,27 +43669,27 @@
       </c>
       <c r="S63" s="3"/>
       <c r="T63">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>1.00505</v>
       </c>
       <c r="U63">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>4.2272922775696388E-3</v>
       </c>
       <c r="Z63" s="10">
-        <f>E26</f>
+        <f t="shared" si="22"/>
         <v>0.85327207875278333</v>
       </c>
       <c r="AA63">
-        <f>M26</f>
+        <f t="shared" si="23"/>
         <v>86.310402678555434</v>
       </c>
       <c r="AB63">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>23.457433510626299</v>
       </c>
       <c r="AC63">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>7.6472342872323535</v>
       </c>
     </row>
@@ -43955,11 +43721,11 @@
         <v>1.0362</v>
       </c>
       <c r="L64">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>1.0322200000000001</v>
       </c>
       <c r="N64">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>5.1036261618578396E-3</v>
       </c>
       <c r="O64">
@@ -43978,27 +43744,27 @@
         <v>1.0085</v>
       </c>
       <c r="T64">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>1.0030999999999999</v>
       </c>
       <c r="U64">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>7.2515515581149884E-3</v>
       </c>
       <c r="Z64" s="10">
-        <f>E27</f>
+        <f t="shared" si="22"/>
         <v>0.87266462599716477</v>
       </c>
       <c r="AA64">
-        <f>M27</f>
+        <f t="shared" si="23"/>
         <v>113.4881509731249</v>
       </c>
       <c r="AB64">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>31.595671506272485</v>
       </c>
       <c r="AC64">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>7.9032315716868959</v>
       </c>
     </row>
@@ -44030,11 +43796,11 @@
         <v>1.0392999999999999</v>
       </c>
       <c r="L65">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>1.03464</v>
       </c>
       <c r="N65">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>7.5834029300835184E-3</v>
       </c>
       <c r="O65">
@@ -44053,27 +43819,27 @@
         <v>1.0135000000000001</v>
       </c>
       <c r="T65">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>1.0104</v>
       </c>
       <c r="U65">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>6.2088646305101594E-3</v>
       </c>
       <c r="Z65" s="10">
-        <f>E28</f>
+        <f t="shared" si="22"/>
         <v>0.8920571732415461</v>
       </c>
       <c r="AA65">
-        <f>M28</f>
+        <f t="shared" si="23"/>
         <v>87.683920431147158</v>
       </c>
       <c r="AB65">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>45.106743368851269</v>
       </c>
       <c r="AC65">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>8.1638921351603919</v>
       </c>
     </row>
@@ -44105,11 +43871,11 @@
         <v>1.0437000000000001</v>
       </c>
       <c r="L66">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>1.03562</v>
       </c>
       <c r="N66">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>1.0307618541641915E-2</v>
       </c>
       <c r="O66">
@@ -44128,27 +43894,27 @@
         <v>1.01</v>
       </c>
       <c r="T66">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>1.0020200000000001</v>
       </c>
       <c r="U66">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>6.2235038362645941E-3</v>
       </c>
       <c r="Z66" s="10">
-        <f>E29</f>
+        <f t="shared" si="22"/>
         <v>0.91144972048592765</v>
       </c>
       <c r="AA66">
-        <f>M29</f>
+        <f t="shared" si="23"/>
         <v>98.537256629245661</v>
       </c>
       <c r="AB66">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>70.072502949490556</v>
       </c>
       <c r="AC66">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>8.4292159776528486</v>
       </c>
     </row>
@@ -44180,11 +43946,11 @@
         <v>1.0461</v>
       </c>
       <c r="L67">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>1.0464199999999999</v>
       </c>
       <c r="N67">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>6.2351423399951474E-3</v>
       </c>
       <c r="O67">
@@ -44203,27 +43969,27 @@
         <v>1.0047999999999999</v>
       </c>
       <c r="T67">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>1.0080800000000001</v>
       </c>
       <c r="U67">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>7.8566532314974791E-3</v>
       </c>
       <c r="Z67" s="10">
-        <f>E30</f>
+        <f t="shared" si="22"/>
         <v>0.93084226773030909</v>
       </c>
       <c r="AA67">
-        <f>M30</f>
+        <f t="shared" si="23"/>
         <v>171.81399366170703</v>
       </c>
       <c r="AB67">
-        <f t="shared" ref="AB67:AB68" si="28">(1-Z67/$AG$52)^(-2)*(1-$AG$53*Z67/$AG$52+$AG$54*(Z67/$AG$52)^2)</f>
+        <f t="shared" ref="AB67:AB68" si="30">(1-Z67/$AG$52)^(-2)*(1-$AG$53*Z67/$AG$52+$AG$54*(Z67/$AG$52)^2)</f>
         <v>124.49668706583786</v>
       </c>
       <c r="AC67">
-        <f t="shared" ref="AC67:AC68" si="29">1+2.5*Z67+6.2*Z67^2</f>
+        <f t="shared" ref="AC67:AC68" si="31">1+2.5*Z67+6.2*Z67^2</f>
         <v>8.6992030991642597</v>
       </c>
     </row>
@@ -44255,11 +44021,11 @@
         <v>1.0455000000000001</v>
       </c>
       <c r="L68">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>1.04714</v>
       </c>
       <c r="N68">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>5.0821255395749861E-3</v>
       </c>
       <c r="O68">
@@ -44278,27 +44044,27 @@
         <v>0.99370000000000003</v>
       </c>
       <c r="T68">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>1.0007000000000001</v>
       </c>
       <c r="U68">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>7.3644415945813479E-3</v>
       </c>
       <c r="Z68" s="10">
-        <f>E31</f>
+        <f t="shared" si="22"/>
         <v>0.95023481497469053</v>
       </c>
       <c r="AA68">
-        <f>M31</f>
+        <f t="shared" si="23"/>
         <v>213.77657409894184</v>
       </c>
       <c r="AB68">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>283.37982938993065</v>
       </c>
       <c r="AC68">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>8.9738534996946289</v>
       </c>
     </row>
@@ -44315,19 +44081,19 @@
         <v>50</v>
       </c>
       <c r="L69" t="e">
-        <f t="shared" ref="L69:L72" si="30">AVERAGE(G69:K69)</f>
+        <f t="shared" ref="L69:L72" si="32">AVERAGE(G69:K69)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="N69" t="e">
-        <f t="shared" ref="N69:N72" si="31">_xlfn.STDEV.S(G69:K69)</f>
+        <f t="shared" ref="N69:N72" si="33">_xlfn.STDEV.S(G69:K69)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="T69" t="e">
-        <f t="shared" ref="T69:T72" si="32">AVERAGE(O69:S69)</f>
+        <f t="shared" ref="T69:T72" si="34">AVERAGE(O69:S69)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="U69" t="e">
-        <f t="shared" ref="U69:U72" si="33">_xlfn.STDEV.S(O69:S69)</f>
+        <f t="shared" ref="U69:U72" si="35">_xlfn.STDEV.S(O69:S69)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Z69" s="10"/>
@@ -44345,19 +44111,19 @@
         <v>51</v>
       </c>
       <c r="L70" t="e">
-        <f t="shared" si="30"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N70" t="e">
-        <f t="shared" si="31"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T70" t="e">
         <f t="shared" si="32"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="N70" t="e">
+        <f t="shared" si="33"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T70" t="e">
+        <f t="shared" si="34"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="U70" t="e">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Z70" s="10"/>
@@ -44375,19 +44141,19 @@
         <v>52</v>
       </c>
       <c r="L71" t="e">
-        <f t="shared" si="30"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N71" t="e">
-        <f t="shared" si="31"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T71" t="e">
         <f t="shared" si="32"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="N71" t="e">
+        <f t="shared" si="33"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T71" t="e">
+        <f t="shared" si="34"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="U71" t="e">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Z71" s="10"/>
@@ -44405,19 +44171,19 @@
         <v>53</v>
       </c>
       <c r="L72" t="e">
-        <f t="shared" si="30"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N72" t="e">
-        <f t="shared" si="31"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T72" t="e">
         <f t="shared" si="32"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="N72" t="e">
+        <f t="shared" si="33"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T72" t="e">
+        <f t="shared" si="34"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="U72" t="e">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Z72" s="10"/>
@@ -44472,4 +44238,59 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Final ver pre cleanup
</commit_message>
<xml_diff>
--- a/Viscosity Testing - Green-Kubo.xlsx
+++ b/Viscosity Testing - Green-Kubo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Particles" sheetId="11" r:id="rId1"/>
@@ -668,6 +668,56 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.1883209397481371"/>
+                  <c:y val="-6.5912073490813645E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:errBars>
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
@@ -1275,6 +1325,7 @@
       <c:valAx>
         <c:axId val="325989136"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -2175,7 +2226,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2768,7 +2818,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2891,7 +2940,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3022,7 +3070,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4477,7 +4524,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4841,7 +4887,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5063,7 +5108,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5427,7 +5471,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5650,7 +5693,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6243,7 +6285,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6366,7 +6407,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6497,7 +6537,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7970,7 +8009,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8334,7 +8372,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -9189,7 +9226,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9553,7 +9589,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -14499,7 +14534,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15181,7 +15215,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -15304,7 +15337,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -28373,8 +28405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T73"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="N33" sqref="N33"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AC9" sqref="AC9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31251,7 +31283,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="L7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AE10" sqref="AE10"/>
     </sheetView>
   </sheetViews>
@@ -34602,7 +34634,7 @@
         <v>0.58177641733144314</v>
       </c>
       <c r="E50">
-        <f t="shared" ref="E40:E73" si="7">L13</f>
+        <f t="shared" ref="E50:E73" si="7">L13</f>
         <v>43.32863227604436</v>
       </c>
       <c r="F50">

</xml_diff>